<commit_message>
finish compiling extractionlogcsv.csv, clean up some folders
</commit_message>
<xml_diff>
--- a/Soil-Data-Raw-R/Soil-Data-RawFolders/Field-Extraction-Log/NCD-extractionlog-janapr2014.xlsx
+++ b/Soil-Data-Raw-R/Soil-Data-RawFolders/Field-Extraction-Log/NCD-extractionlog-janapr2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15500" yWindow="0" windowWidth="18080" windowHeight="17860" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="1120" windowWidth="18080" windowHeight="17860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -190,6 +190,30 @@
           </rPr>
           <t xml:space="preserve">
 Note that I didn't actually write down at the time what bag size I used for the dates prior to 1/7/2013… I just tried to remember (it certainly wasn't a big bag, so only medium or large are options) and also asked Adilson.  Add to that the fact that I only used the medium bags once right after visiting home for a week and I feel at least somewhat confident that all the early dates I used small bags.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A64" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Christine O'Connell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+these were S3 (see NCD GPS Points excel doc and field notebook for that day)</t>
         </r>
       </text>
     </comment>
@@ -8452,10 +8476,10 @@
   <dimension ref="A1:AK323"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="6" topLeftCell="G38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="A64" sqref="A64:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -31426,15 +31450,15 @@
         <v>48</v>
       </c>
       <c r="J296" s="86">
-        <f>G296-$J$3</f>
+        <f t="shared" ref="J296:J305" si="77">G296-$J$3</f>
         <v>180.79</v>
       </c>
       <c r="K296" s="43">
-        <f t="shared" ref="K296:K309" si="77">H296-2.41</f>
+        <f t="shared" ref="K296:K309" si="78">H296-2.41</f>
         <v>134.79</v>
       </c>
       <c r="L296" s="39">
-        <f t="shared" ref="L296:L309" si="78">J296-K296</f>
+        <f t="shared" ref="L296:L309" si="79">J296-K296</f>
         <v>46</v>
       </c>
       <c r="M296" s="54">
@@ -31506,15 +31530,15 @@
         <v>48</v>
       </c>
       <c r="J297" s="86">
-        <f>G297-$J$3</f>
+        <f t="shared" si="77"/>
         <v>189.46</v>
       </c>
       <c r="K297" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>139.19</v>
       </c>
       <c r="L297" s="39">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>50.27000000000001</v>
       </c>
       <c r="M297" s="54">
@@ -31586,15 +31610,15 @@
         <v>48</v>
       </c>
       <c r="J298" s="86">
-        <f>G298-$J$3</f>
+        <f t="shared" si="77"/>
         <v>136.84</v>
       </c>
       <c r="K298" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>101.19</v>
       </c>
       <c r="L298" s="39">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>35.650000000000006</v>
       </c>
       <c r="M298" s="54">
@@ -31666,15 +31690,15 @@
         <v>48</v>
       </c>
       <c r="J299" s="86">
-        <f>G299-$J$3</f>
+        <f t="shared" si="77"/>
         <v>87.7</v>
       </c>
       <c r="K299" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>63.790000000000006</v>
       </c>
       <c r="L299" s="39">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>23.909999999999997</v>
       </c>
       <c r="M299" s="54">
@@ -31746,15 +31770,15 @@
         <v>48</v>
       </c>
       <c r="J300" s="86">
-        <f>G300-$J$3</f>
+        <f t="shared" si="77"/>
         <v>151.62</v>
       </c>
       <c r="K300" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>112.29</v>
       </c>
       <c r="L300" s="39">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>39.33</v>
       </c>
       <c r="M300" s="54">
@@ -31826,11 +31850,11 @@
         <v>48</v>
       </c>
       <c r="J301" s="86">
-        <f>G301-$J$3</f>
+        <f t="shared" si="77"/>
         <v>134.09</v>
       </c>
       <c r="K301" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>110.99000000000001</v>
       </c>
       <c r="L301" s="39">
@@ -31906,11 +31930,11 @@
         <v>48</v>
       </c>
       <c r="J302" s="86">
-        <f>G302-$J$3</f>
+        <f t="shared" si="77"/>
         <v>169.26</v>
       </c>
       <c r="K302" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>141.89000000000001</v>
       </c>
       <c r="L302" s="39">
@@ -31986,11 +32010,11 @@
         <v>48</v>
       </c>
       <c r="J303" s="86">
-        <f>G303-$J$3</f>
+        <f t="shared" si="77"/>
         <v>126.03999999999999</v>
       </c>
       <c r="K303" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>102.49000000000001</v>
       </c>
       <c r="L303" s="39">
@@ -32068,11 +32092,11 @@
         <v>48</v>
       </c>
       <c r="J304" s="86">
-        <f>G304-$J$3</f>
+        <f t="shared" si="77"/>
         <v>119.28999999999999</v>
       </c>
       <c r="K304" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>98.59</v>
       </c>
       <c r="L304" s="39">
@@ -32148,11 +32172,11 @@
         <v>48</v>
       </c>
       <c r="J305" s="86">
-        <f>G305-$J$3</f>
+        <f t="shared" si="77"/>
         <v>104.67999999999999</v>
       </c>
       <c r="K305" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>87.19</v>
       </c>
       <c r="L305" s="39">
@@ -32228,15 +32252,15 @@
         <v>48</v>
       </c>
       <c r="J306" s="86">
-        <f t="shared" ref="J296:J309" si="79">G306-$J$3</f>
+        <f t="shared" ref="J306:J309" si="80">G306-$J$3</f>
         <v>124.50999999999999</v>
       </c>
       <c r="K306" s="43">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>98.79</v>
       </c>
       <c r="L306" s="39">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>25.719999999999985</v>
       </c>
       <c r="M306" s="54">
@@ -32308,15 +32332,15 @@
         <v>48</v>
       </c>
       <c r="J307" s="86">
+        <f t="shared" si="80"/>
+        <v>115.38</v>
+      </c>
+      <c r="K307" s="43">
+        <f t="shared" si="78"/>
+        <v>89.59</v>
+      </c>
+      <c r="L307" s="39">
         <f t="shared" si="79"/>
-        <v>115.38</v>
-      </c>
-      <c r="K307" s="43">
-        <f t="shared" si="77"/>
-        <v>89.59</v>
-      </c>
-      <c r="L307" s="39">
-        <f t="shared" si="78"/>
         <v>25.789999999999992</v>
       </c>
       <c r="M307" s="54">
@@ -32388,15 +32412,15 @@
         <v>48</v>
       </c>
       <c r="J308" s="86">
+        <f t="shared" si="80"/>
+        <v>113.57</v>
+      </c>
+      <c r="K308" s="43">
+        <f t="shared" si="78"/>
+        <v>89.19</v>
+      </c>
+      <c r="L308" s="39">
         <f t="shared" si="79"/>
-        <v>113.57</v>
-      </c>
-      <c r="K308" s="43">
-        <f t="shared" si="77"/>
-        <v>89.19</v>
-      </c>
-      <c r="L308" s="39">
-        <f t="shared" si="78"/>
         <v>24.379999999999995</v>
       </c>
       <c r="M308" s="54">
@@ -32468,15 +32492,15 @@
         <v>48</v>
       </c>
       <c r="J309" s="86">
+        <f t="shared" si="80"/>
+        <v>127.31</v>
+      </c>
+      <c r="K309" s="43">
+        <f t="shared" si="78"/>
+        <v>100.49000000000001</v>
+      </c>
+      <c r="L309" s="39">
         <f t="shared" si="79"/>
-        <v>127.31</v>
-      </c>
-      <c r="K309" s="43">
-        <f t="shared" si="77"/>
-        <v>100.49000000000001</v>
-      </c>
-      <c r="L309" s="39">
-        <f t="shared" si="78"/>
         <v>26.819999999999993</v>
       </c>
       <c r="M309" s="54">
@@ -32893,15 +32917,15 @@
         <v>48</v>
       </c>
       <c r="J315" s="86">
-        <f t="shared" ref="J315:J318" si="80">G315-$J$3</f>
+        <f t="shared" ref="J315:J318" si="81">G315-$J$3</f>
         <v>115.19</v>
       </c>
       <c r="K315" s="43">
-        <f t="shared" ref="K315:K318" si="81">H315-2.41</f>
+        <f t="shared" ref="K315:K318" si="82">H315-2.41</f>
         <v>92.09</v>
       </c>
       <c r="L315" s="39">
-        <f t="shared" ref="L315:L318" si="82">J315-K315</f>
+        <f t="shared" ref="L315:L318" si="83">J315-K315</f>
         <v>23.099999999999994</v>
       </c>
       <c r="M315" s="54">
@@ -32973,15 +32997,15 @@
         <v>48</v>
       </c>
       <c r="J316" s="86">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>111.06</v>
       </c>
       <c r="K316" s="43">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>88.990000000000009</v>
       </c>
       <c r="L316" s="39">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>22.069999999999993</v>
       </c>
       <c r="M316" s="54">
@@ -33053,15 +33077,15 @@
         <v>48</v>
       </c>
       <c r="J317" s="86">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>143.69999999999999</v>
       </c>
       <c r="K317" s="43">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>113.19</v>
       </c>
       <c r="L317" s="39">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>30.509999999999991</v>
       </c>
       <c r="M317" s="54">
@@ -33133,15 +33157,15 @@
         <v>48</v>
       </c>
       <c r="J318" s="86">
-        <f t="shared" si="80"/>
+        <f t="shared" si="81"/>
         <v>129.28</v>
       </c>
       <c r="K318" s="43">
-        <f t="shared" si="81"/>
+        <f t="shared" si="82"/>
         <v>104.29</v>
       </c>
       <c r="L318" s="39">
-        <f t="shared" si="82"/>
+        <f t="shared" si="83"/>
         <v>24.989999999999995</v>
       </c>
       <c r="M318" s="54">

</xml_diff>